<commit_message>
update film dim ,ssas, pbi supermarket, mdx supermarket
</commit_message>
<xml_diff>
--- a/NEW DATASET/film_sales.xlsx
+++ b/NEW DATASET/film_sales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK1_4\BI\BI.07_Project\NEW DATASET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8298b686301d6f78/Máy tính/BI07_Nhom/BI.07_Project/NEW DATASET/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A4FCC0-B8E2-4B55-B99B-D09B94968C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A7A4FCC0-B8E2-4B55-B99B-D09B94968C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C108AC62-7138-4B77-B6B1-A8792084A02A}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="2388" windowWidth="15852" windowHeight="9972" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9456" yWindow="2544" windowWidth="12648" windowHeight="9696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Film" sheetId="2" r:id="rId1"/>
@@ -1136,8 +1136,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1212,7 +1212,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1316,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1557D15E-5BEF-44FA-8020-56F564CF42F8}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>